<commit_message>
Numpad not working, no pop-ups
27 needs a bit of work.
Fix numpad functionality.
Fix SAN text input pop-up.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="4.2_Items" sheetId="1" state="visible" r:id="rId1"/>
@@ -282,7 +282,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,10 +314,10 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
+        <v>152</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>1152</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>902</v>
       </c>
     </row>
     <row r="3" ht="24" customHeight="1" s="4">
@@ -327,10 +327,10 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
+        <v>408</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>1408</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>1433</v>
       </c>
     </row>
     <row r="4" ht="24" customHeight="1" s="4">
@@ -497,10 +497,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -1181,46 +1181,20 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2023-12-08 00:25:38</t>
+          <t>2023-12-08 00:41:11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Dock Thunderbolt G4</t>
+          <t>Laptop 840 G9</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Add 25</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2023-12-08 00:25:51</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Desktop Mini</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Subtract 250</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>54321</t>
-        </is>
-      </c>
+          <t>Add 2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1243,14 +1217,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>LastCount</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>NewCount</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1271,10 +1263,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -1282,66 +1274,22 @@
     <row r="1" ht="12.75" customHeight="1" s="4">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>2023-12-08 00:14:21</t>
+          <t>Timestamp</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wireless Headset Poly </t>
+          <t>Item</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>Add 5</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-08 00:25:38</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Dock Thunderbolt G4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Add 25</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-08 00:25:51</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Desktop Mini</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Subtract 250</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>54321</t>
+          <t>SAN Number</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the logic for SAN#
This code now includes the SANInputDialog class, which will prompt for a numeric input and return a string prefixed with "SAN". The update_count function has been modified to check if the selected item is a "laptop" or "mini-pc" and, if so, to use the SANInputDialog to get the SAN number. This number is then logged and saved in the spreadsheet.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -314,10 +314,10 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>152</v>
+        <v>1153</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>1152</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="3" ht="24" customHeight="1" s="4">
@@ -327,10 +327,10 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>1409</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="4" ht="24" customHeight="1" s="4">
@@ -340,10 +340,10 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>40</v>
+        <v>940</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>1040</v>
+        <v>990</v>
       </c>
     </row>
     <row r="5" ht="24" customHeight="1" s="4">
@@ -353,10 +353,10 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" ht="24" customHeight="1" s="4">
@@ -382,7 +382,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" ht="24" customHeight="1" s="4">
@@ -392,10 +392,10 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>11</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" ht="24" customHeight="1" s="4">
@@ -431,10 +431,10 @@
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>40</v>
+        <v>78040</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>78040</v>
+        <v>78020</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" s="4">
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1308,40 +1308,190 @@
       <c r="D46" s="3" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="3" t="inlineStr">
         <is>
           <t>2023-12-08 22:51:31</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="3" t="inlineStr">
         <is>
           <t>Add 2</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
+      <c r="D47" s="3" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="3" t="inlineStr">
         <is>
           <t>2023-12-08 22:51:37</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="3" t="inlineStr">
         <is>
           <t>USB External DVD-RW Drive</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="3" t="inlineStr">
         <is>
           <t>Add 7</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" s="3" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:35:08</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="inlineStr">
+        <is>
+          <t>Add 5000</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:45:46</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 68</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:46:04</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-12-09 21:43:21</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Add 2</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-12-09 21:43:25</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Add 2</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-12-09 21:43:31</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-12-09 21:43:49</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-12-09 21:45:37</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Add 3</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>SAN111</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1398,6 +1548,12 @@
           <t>Desktop Mini</t>
         </is>
       </c>
+      <c r="B2" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" ht="35.5" customHeight="1" s="4">
       <c r="A3" s="5" t="inlineStr">
@@ -1405,6 +1561,12 @@
           <t>Dock Thunderbolt G4</t>
         </is>
       </c>
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" ht="24.05" customHeight="1" s="4">
       <c r="A4" s="5" t="inlineStr">
@@ -1412,6 +1574,12 @@
           <t>Laptop 840 G10</t>
         </is>
       </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" ht="24.05" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -1419,6 +1587,12 @@
           <t>Laptop 840 G9</t>
         </is>
       </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" ht="24.05" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -1426,6 +1600,12 @@
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" ht="24.05" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -1433,12 +1613,21 @@
           <t>Laptop x360 G8</t>
         </is>
       </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="4">
       <c r="A8" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Monitor 24” </t>
         </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>11143</v>
       </c>
     </row>
     <row r="9" ht="24.05" customHeight="1" s="4">
@@ -1504,7 +1693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1598,19 +1787,88 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>2023-12-08 22:51:23</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:35:20</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:35:23</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Add 5000</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:45:11</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 23</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-08 23:45:29</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 68</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified the show_san_input function
Modified the show_san-input function so that the while True loop will continuously display the SAN input dialog until the user enters a valid SAN number that meets the length requirement. If the user enters an invalid SAN number (less than 5 characters), an error message is shown, and the dialog is displayed again.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -328,10 +328,10 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" ht="24" customHeight="1" s="4">
@@ -340,8 +340,12 @@
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" ht="24" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -350,10 +354,10 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" ht="24" customHeight="1" s="4">
@@ -467,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -996,24 +1000,134 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
+      <c r="A84" s="3" t="inlineStr">
         <is>
           <t>2023-12-11 20:10:38</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" s="3" t="inlineStr">
         <is>
           <t>Desktop Mini</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C84" s="3" t="inlineStr">
         <is>
           <t>Add 1</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="D84" s="3" t="inlineStr">
         <is>
           <t>22222</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:28:29</t>
+        </is>
+      </c>
+      <c r="B85" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C85" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:28:32</t>
+        </is>
+      </c>
+      <c r="B86" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C86" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="inlineStr">
+        <is>
+          <t>55555</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:32:27</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>33333</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:32:33</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>33333</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:32:45</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>44444</t>
         </is>
       </c>
     </row>
@@ -1090,8 +1204,12 @@
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" ht="24" customHeight="1" s="4">
       <c r="A5" s="5" t="inlineStr">
@@ -1099,8 +1217,12 @@
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" ht="24" customHeight="1" s="4">
       <c r="A6" s="5" t="inlineStr">
@@ -1212,7 +1334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1283,6 +1405,28 @@
     </row>
     <row r="16" ht="12.75" customHeight="1" s="4">
       <c r="D16" s="3" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:28:50</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
Treeview 8 rows, descending order
The log_view Treeview is set to display 8 rows at a time (height=8), and the scrollbar allows you to scroll through all the rows. The entries in the log_view are sorted in descending order, showing the most recent entries first
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -315,10 +315,10 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" ht="24" customHeight="1" s="4">
@@ -366,8 +366,12 @@
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
+      <c r="B6" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" ht="24" customHeight="1" s="4">
       <c r="A7" s="5" t="inlineStr">
@@ -384,8 +388,12 @@
           <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" ht="24" customHeight="1" s="4">
       <c r="A9" s="5" t="inlineStr">
@@ -393,8 +401,12 @@
           <t>Monitor 34” Ultrawide</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>-2</v>
+      </c>
     </row>
     <row r="10" ht="35.25" customHeight="1" s="4">
       <c r="A10" s="5" t="inlineStr">
@@ -402,8 +414,12 @@
           <t>USB External DVD-RW Drive</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
+      <c r="B10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" s="4">
       <c r="A11" s="5" t="inlineStr">
@@ -411,8 +427,12 @@
           <t>Wired Headset Poly 3325</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" s="4">
       <c r="A12" s="5" t="inlineStr">
@@ -438,8 +458,12 @@
           <t xml:space="preserve">Wireless Headset Poly </t>
         </is>
       </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" ht="24" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -471,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1066,68 +1090,288 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="3" t="inlineStr">
         <is>
           <t>2023-12-11 20:32:27</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Add 1</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
+      <c r="C87" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="inlineStr">
         <is>
           <t>33333</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="A88" s="3" t="inlineStr">
         <is>
           <t>2023-12-11 20:32:33</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B88" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Add 1</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
+      <c r="C88" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="inlineStr">
         <is>
           <t>33333</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="3" t="inlineStr">
         <is>
           <t>2023-12-11 20:32:45</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B89" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Add 1</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
+      <c r="C89" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="inlineStr">
         <is>
           <t>44444</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:35:47</t>
+        </is>
+      </c>
+      <c r="B90" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C90" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="inlineStr">
+        <is>
+          <t>33333</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:35:50</t>
+        </is>
+      </c>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="inlineStr">
+        <is>
+          <t>44444</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 20:35:54</t>
+        </is>
+      </c>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
+          <t>df333</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:13:40</t>
+        </is>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:17:43</t>
+        </is>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>44444</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:17:46</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>55555</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:17:49</t>
+        </is>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>66666</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:01</t>
+        </is>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>44444</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:06</t>
+        </is>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>44444</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 22:15:53</t>
+        </is>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>22222</t>
         </is>
       </c>
     </row>
@@ -1283,8 +1527,12 @@
           <t>Wired Keyboard</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
+      <c r="B12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" s="4">
       <c r="A13" s="5" t="inlineStr">
@@ -1301,8 +1549,12 @@
           <t xml:space="preserve">Wireless Headset Poly </t>
         </is>
       </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>-400</v>
+      </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -1310,8 +1562,12 @@
           <t>Wireless Keyboard and Mouse</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n"/>
-      <c r="C15" s="3" t="n"/>
+      <c r="B15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>400</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1334,7 +1590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1425,6 +1681,160 @@
       <c r="D17" s="3" t="inlineStr">
         <is>
           <t>22222</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:15</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>sasdfadsdas</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:20</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>53455534</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:21</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>345345</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:23</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>345345345</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 21:18:25</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>45345345</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 22:43:32</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-11 22:43:36</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>33333</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Custom validation function to allow only numeric input
Only numerals allowed as input
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -318,10 +318,10 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>63</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>64</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="4">
@@ -531,7 +531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1372,82 +1372,100 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="3" t="inlineStr">
         <is>
           <t>Add 1</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr">
+      <c r="C41" s="3" t="inlineStr"/>
+      <c r="D41" s="3" t="inlineStr">
         <is>
           <t>2023-12-27 20:56:56</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="3" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="3" t="inlineStr">
         <is>
           <t>SAN2323233</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="3" t="inlineStr">
         <is>
           <t>2023-12-27 20:57:04</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
         <is>
           <t>Add 1</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr">
+      <c r="C43" s="3" t="inlineStr"/>
+      <c r="D43" s="3" t="inlineStr">
         <is>
           <t>2023-12-27 20:58:06</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="3" t="inlineStr">
         <is>
           <t>SAN333333</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="3" t="inlineStr">
         <is>
           <t>2023-12-27 20:58:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Subtract 1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2023-12-28 14:01:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update_count function and the section where the "All SANs" sheet is appended
These changes ensure that the log is written in the correct order and that the log view is refreshed immediately after each operation, displaying the entries sorted by the timestamp in descending order ("newest first"). Additionally, it corrects the order of data appended to the "All SANs" sheet.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -337,10 +337,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="6">
@@ -555,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
@@ -788,139 +788,203 @@
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="6">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>SAN111233</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:13:14</t>
         </is>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="6">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>SAN232323</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:13:29</t>
         </is>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="6">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>SAN121211</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:16:49</t>
         </is>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="6">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>SAN676867</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:16:55</t>
         </is>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="6">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="5" t="inlineStr">
         <is>
           <t>SAN134578</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:17:36</t>
         </is>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="6">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>SAN777987</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:17:51</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="12.75" customHeight="1" s="6"/>
-    <row r="18" ht="12.75" customHeight="1" s="6"/>
+    <row r="17" ht="12.75" customHeight="1" s="6">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>SAN888444</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:20:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="6">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>SAN555555</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:21:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>SAN344556</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:32:03</t>
+        </is>
+      </c>
+    </row>
     <row r="1048576" ht="12.75" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -978,10 +1042,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="6">
@@ -1188,7 +1252,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
@@ -1222,9 +1286,72 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12" customHeight="1" s="6"/>
-    <row r="3" ht="12.75" customHeight="1" s="6"/>
-    <row r="4" ht="12.75" customHeight="1" s="6"/>
+    <row r="2" ht="12" customHeight="1" s="6">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="6">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SAN454545</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="6">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SAN535353</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:13</t>
+        </is>
+      </c>
+    </row>
     <row r="5" ht="12.75" customHeight="1" s="6"/>
     <row r="6" ht="12.75" customHeight="1" s="6"/>
     <row r="7" ht="12.75" customHeight="1" s="6"/>
@@ -1502,7 +1629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
@@ -1684,113 +1811,209 @@
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="6">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>SAN111233</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:13:14</t>
         </is>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="6">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>SAN232323</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:13:29</t>
         </is>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="6">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>SAN121211</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:16:49</t>
         </is>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="6">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>SAN676867</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:16:55</t>
         </is>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="6">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>SAN134578</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:17:36</t>
         </is>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="6">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>SAN777987</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>2023-12-28 23:17:51</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="12.75" customHeight="1" s="6"/>
-    <row r="18" ht="12.75" customHeight="1" s="6"/>
-    <row r="19" ht="12.75" customHeight="1" s="6"/>
-    <row r="20" ht="12.75" customHeight="1" s="6"/>
-    <row r="21" ht="12.75" customHeight="1" s="6"/>
-    <row r="22" ht="12.75" customHeight="1" s="6"/>
+    <row r="17" ht="12.75" customHeight="1" s="6">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>SAN888444</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:20:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="6">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>SAN555555</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:21:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1" s="6">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>SAN344556</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-28 23:32:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="6">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SAN454545</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="12.75" customHeight="1" s="6">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SAN535353</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:07:13</t>
+        </is>
+      </c>
+    </row>
     <row r="23" ht="12.75" customHeight="1" s="6"/>
     <row r="24" ht="12.75" customHeight="1" s="6"/>
     <row r="25" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Only items with G8, G9 or G10 in their names should trigger the SAN Input fuction
If no SAN, update the count in the Items sheet
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="4.2 Items" sheetId="1" state="visible" r:id="rId1"/>
@@ -303,7 +303,7 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -337,10 +337,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="6">
@@ -376,10 +376,10 @@
         </is>
       </c>
       <c r="B5" s="7" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" ht="24" customHeight="1" s="6">
@@ -389,10 +389,10 @@
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" ht="24" customHeight="1" s="6">
@@ -402,7 +402,7 @@
         </is>
       </c>
       <c r="B7" s="7" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>32</v>
@@ -415,10 +415,10 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="24" customHeight="1" s="6">
@@ -428,10 +428,10 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" ht="24" customHeight="1" s="6">
@@ -464,9 +464,11 @@
           <t>USB DVD-RW Drive</t>
         </is>
       </c>
-      <c r="B12" s="7" t="n"/>
+      <c r="B12" s="7" t="n">
+        <v>9</v>
+      </c>
       <c r="C12" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" s="6">
@@ -515,10 +517,10 @@
         </is>
       </c>
       <c r="B16" s="7" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C16" s="7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" ht="24" customHeight="1" s="6">
@@ -555,15 +557,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="14.56" customWidth="1" style="5" min="1" max="1"/>
+    <col width="18.29" customWidth="1" style="5" min="1" max="1"/>
+    <col width="20.52" customWidth="1" style="5" min="2" max="2"/>
     <col width="18.22" customWidth="1" style="5" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -592,396 +595,572 @@
     <row r="2" ht="12.75" customHeight="1" s="6">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 13:04:00</t>
         </is>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>SAN232323</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:34:09</t>
+          <t>SAN123456</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 13:04:08</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:37:58</t>
+          <t>SAN11111</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="6">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 21:57:18</t>
         </is>
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:01</t>
+          <t>SAN123654</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="6">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 21:57:29</t>
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>SAN87878</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:03</t>
+          <t>SAN111222</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 22:03:45</t>
         </is>
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>SAN787878</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:05</t>
+          <t>SAN111122</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="6">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 22:03:49</t>
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:08</t>
+          <t>SAN123212</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="6">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>2023-12-29 22:04:05</t>
         </is>
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>SAN222223</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:05:29</t>
+          <t>SAN111111</t>
         </is>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="6">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>2023-12-29 22:04:20</t>
         </is>
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>SAN333333</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:05:45</t>
+          <t>SAN132433</t>
         </is>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="6">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 22:34:24</t>
         </is>
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>SAN111111</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:06:58</t>
+          <t>SAN258741</t>
         </is>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="6">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 22:34:28</t>
         </is>
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>SAN111233</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:13:14</t>
+          <t>SAN789654</t>
         </is>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="6">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 22:40:56</t>
         </is>
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>SAN232323</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:13:29</t>
+          <t>SAN987456</t>
         </is>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="6">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 22:41:01</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>SAN121211</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:16:49</t>
+          <t>SAN321654</t>
         </is>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="6">
       <c r="A14" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 23:41:50</t>
         </is>
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>SAN676867</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D14" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:16:55</t>
+          <t>SAN111111</t>
         </is>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="6">
       <c r="A15" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 23:41:55</t>
         </is>
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>SAN134578</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:17:36</t>
+          <t>SAN545545</t>
         </is>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="6">
       <c r="A16" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>2023-12-29 23:44:47</t>
         </is>
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>SAN777987</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D16" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:17:51</t>
+          <t>SAN789456</t>
         </is>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="6">
       <c r="A17" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 23:44:52</t>
         </is>
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>SAN888444</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:20:29</t>
+          <t>SAN456789</t>
         </is>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" s="6">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 23:55:58</t>
         </is>
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>USB DVD-RW Drive</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>SAN555555</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:21:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
+          <t>SAN454545</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1" s="6">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>2023-12-29 23:56:02</t>
         </is>
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>USB DVD-RW Drive</t>
         </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>SAN344556</t>
+          <t>add</t>
         </is>
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:32:03</t>
+          <t>SAN121212</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-30 22:52:47</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>SAN554544</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="12.75" customHeight="1" s="6">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:29:57</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>SAN456123</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="12.75" customHeight="1" s="6">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:30:30</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>SAN444555</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="12.75" customHeight="1" s="6">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:10</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>SAN456665</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="12.75" customHeight="1" s="6">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:19</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>SAN444444</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="12.75" customHeight="1" s="6">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:27</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>SAN453212</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:50:20</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 11:33:44</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>SAN111111</t>
         </is>
       </c>
     </row>
@@ -1042,10 +1221,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="6">
@@ -1094,10 +1273,10 @@
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" ht="24" customHeight="1" s="6">
@@ -1252,10 +1431,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1286,84 +1465,364 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12" customHeight="1" s="6">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SAN343434</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" s="6">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="6">
+      <c r="A2" s="7" t="n"/>
+      <c r="B2" s="7" t="n"/>
+      <c r="C2" s="7" t="n"/>
+      <c r="D2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="12" customHeight="1" s="6">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:04:25</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>SAN456456</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="6">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:04:28</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>SAN123123</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="6">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:37</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>SAN147896</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:37</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>SAN444555</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="6">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:37</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>SAN111254</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="6">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:37</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>SAN777778</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="6">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:37</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>SAN555888</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="6">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:41</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>SAN747474</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="6">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:44</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>SAN47474</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="6">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:45</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>SAN47474</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="6">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:47</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>SAN47474</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1" s="6">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 13:48:49</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>SAN47474</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1" s="6">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 23:42:08</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>SAN545454</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="12.75" customHeight="1" s="6">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-29 23:42:10</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>SAN454545</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="6">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SAN535353</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1" s="6"/>
-    <row r="6" ht="12.75" customHeight="1" s="6"/>
-    <row r="7" ht="12.75" customHeight="1" s="6"/>
-    <row r="8" ht="12.75" customHeight="1" s="6"/>
-    <row r="9" ht="12.75" customHeight="1" s="6"/>
-    <row r="10" ht="12.75" customHeight="1" s="6"/>
-    <row r="11" ht="12.75" customHeight="1" s="6"/>
-    <row r="12" ht="12.75" customHeight="1" s="6"/>
-    <row r="13" ht="12.75" customHeight="1" s="6"/>
-    <row r="14" ht="12.75" customHeight="1" s="6"/>
-    <row r="15" ht="12.75" customHeight="1" s="6"/>
-    <row r="1048576" ht="12.75" customHeight="1" s="6"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1" s="6">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-30 00:32:09</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>SAN159789</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="6">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-30 00:32:13</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1629,10 +2088,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1640,7 +2099,7 @@
     <col width="25.36" customWidth="1" style="5" min="1" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customFormat="1" customHeight="1" s="9">
+    <row r="1" ht="12.75" customHeight="1" s="6">
       <c r="A1" s="9" t="inlineStr">
         <is>
           <t>SAN Number</t>
@@ -1660,360 +2119,136 @@
     <row r="2" ht="12.75" customHeight="1" s="6">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>SAN232323</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>SAN456123</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:34:09</t>
+          <t>2023-12-31 10:29:57</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>Laptop x360 G8</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>SAN444555</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:37:58</t>
+          <t>2023-12-31 10:30:30</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="6">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>Dock Thunderbolt G4</t>
         </is>
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>SAN456665</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:01</t>
+          <t>2023-12-31 10:31:10</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="6">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>SAN87878</t>
+          <t xml:space="preserve">Wireless Headset Poly </t>
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>SAN444444</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:03</t>
+          <t>2023-12-31 10:31:19</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>SAN787878</t>
+          <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>SAN453212</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:05</t>
+          <t>2023-12-31 10:31:27</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="6">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>SAN878787</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>SAN343434</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 22:38:08</t>
+          <t>2023-12-31 10:50:20</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="6">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>SAN222223</t>
+          <t>SAN111111</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>2023-12-28 23:05:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="6">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>SAN333333</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:05:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1" s="6">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>SAN111111</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:06:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1" s="6">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>SAN111233</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:13:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1" s="6">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>SAN232323</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:13:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1" s="6">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>SAN121211</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:16:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1" s="6">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>SAN676867</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:16:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1" s="6">
-      <c r="A15" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>SAN134578</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:17:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1" s="6">
-      <c r="A16" s="5" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="B16" s="5" t="inlineStr">
-        <is>
-          <t>SAN777987</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:17:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1" s="6">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>SAN888444</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:20:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1" s="6">
-      <c r="A18" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>SAN555555</t>
-        </is>
-      </c>
-      <c r="C18" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:21:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="12.75" customHeight="1" s="6">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B19" s="5" t="inlineStr">
-        <is>
-          <t>SAN344556</t>
-        </is>
-      </c>
-      <c r="C19" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-28 23:32:03</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="12.75" customHeight="1" s="6">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SAN343434</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="12.75" customHeight="1" s="6">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SAN454545</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="12.75" customHeight="1" s="6">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>SAN535353</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2023-12-29 00:07:13</t>
-        </is>
-      </c>
-    </row>
+          <t>2023-12-31 11:33:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="6"/>
+    <row r="10" ht="12.75" customHeight="1" s="6"/>
+    <row r="11" ht="12.75" customHeight="1" s="6"/>
+    <row r="12" ht="12.75" customHeight="1" s="6"/>
+    <row r="13" ht="12.75" customHeight="1" s="6"/>
+    <row r="14" ht="12.75" customHeight="1" s="6"/>
+    <row r="15" ht="12.75" customHeight="1" s="6"/>
+    <row r="16" ht="12.75" customHeight="1" s="6"/>
+    <row r="17" ht="12.75" customHeight="1" s="6"/>
+    <row r="18" ht="12.75" customHeight="1" s="6"/>
+    <row r="19" ht="12.75" customHeight="1" s="6"/>
+    <row r="20" ht="12.75" customHeight="1" s="6"/>
+    <row r="21" ht="12.75" customHeight="1" s="6"/>
+    <row r="22" ht="12.75" customHeight="1" s="6"/>
     <row r="23" ht="12.75" customHeight="1" s="6"/>
     <row r="24" ht="12.75" customHeight="1" s="6"/>
     <row r="25" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Updated update_count function - when subtracting, it checks if the SAN exists in the "All SANs" sheet.
 If it does, the SAN is removed from the sheet. If the SAN does not exist, an error message is displayed. This ensures that the subtraction of items with SANs is handled correctly according to the specified logic.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -337,10 +337,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1" s="6">
@@ -363,10 +363,10 @@
         </is>
       </c>
       <c r="B4" s="7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="24" customHeight="1" s="6">
@@ -405,7 +405,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" ht="24" customHeight="1" s="6">
@@ -557,7 +557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1159,6 +1159,138 @@
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>SAN111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:35:48</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>SAN122334</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:36:48</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>SAN222211</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>SAN456789</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>SAN125689</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:57</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>SAN357895</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-12-31 14:20:35</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>SAN111111</t>
         </is>
@@ -2088,7 +2220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -2226,19 +2358,83 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>SAN111111</t>
+          <t>SAN122334</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>2023-12-31 11:33:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="6"/>
-    <row r="10" ht="12.75" customHeight="1" s="6"/>
-    <row r="11" ht="12.75" customHeight="1" s="6"/>
-    <row r="12" ht="12.75" customHeight="1" s="6"/>
+          <t>2023-12-31 12:35:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="6">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>SAN222211</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:36:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="6">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>SAN456789</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="6">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>SAN125689</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="6">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>SAN357895</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:57</t>
+        </is>
+      </c>
+    </row>
     <row r="13" ht="12.75" customHeight="1" s="6"/>
     <row r="14" ht="12.75" customHeight="1" s="6"/>
     <row r="15" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Order of columns sorted
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="4.2 Items" sheetId="1" state="visible" r:id="rId1"/>
@@ -304,10 +304,10 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -330,33 +330,33 @@
       </c>
       <c r="D1" s="5" t="n"/>
     </row>
-    <row r="2" ht="46.5" customHeight="1" s="6">
+    <row r="2" ht="12.75" customHeight="1" s="6">
       <c r="A2" s="8" t="inlineStr">
         <is>
           <t>Desktop Mini G9</t>
         </is>
       </c>
       <c r="B2" s="7" t="n">
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="n">
         <v>110</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" ht="46.5" customHeight="1" s="6">
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="6">
       <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" ht="46.5" customHeight="1" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="6">
       <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G2</t>
@@ -369,7 +369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="24" customHeight="1" s="6">
+    <row r="5" ht="12.75" customHeight="1" s="6">
       <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G4</t>
@@ -382,7 +382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" ht="24" customHeight="1" s="6">
+    <row r="6" ht="12.75" customHeight="1" s="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
@@ -395,7 +395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" ht="24" customHeight="1" s="6">
+    <row r="7" ht="12.75" customHeight="1" s="6">
       <c r="A7" s="8" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
@@ -408,7 +408,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="24" customHeight="1" s="6">
+    <row r="8" ht="12.75" customHeight="1" s="6">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Laptop Charger </t>
@@ -421,7 +421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" ht="24" customHeight="1" s="6">
+    <row r="9" ht="12.75" customHeight="1" s="6">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
@@ -434,7 +434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="24" customHeight="1" s="6">
+    <row r="10" ht="12.75" customHeight="1" s="6">
       <c r="A10" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Monitor 24” </t>
@@ -447,18 +447,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" ht="24" customHeight="1" s="6">
+    <row r="11" ht="12.75" customHeight="1" s="6">
       <c r="A11" s="8" t="inlineStr">
         <is>
           <t>Monitor 34” Ultrawide</t>
         </is>
       </c>
-      <c r="B11" s="7" t="n"/>
+      <c r="B11" s="7" t="n">
+        <v>11</v>
+      </c>
       <c r="C11" s="7" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" ht="35.25" customHeight="1" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="6">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>USB DVD-RW Drive</t>
@@ -471,7 +473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" ht="35.25" customHeight="1" s="6">
+    <row r="13" ht="12.75" customHeight="1" s="6">
       <c r="A13" s="8" t="inlineStr">
         <is>
           <t>Wired Headset Poly</t>
@@ -484,7 +486,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" ht="35.25" customHeight="1" s="6">
+    <row r="14" ht="12.75" customHeight="1" s="6">
       <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Wired Keyboard</t>
@@ -497,7 +499,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" ht="35.25" customHeight="1" s="6">
+    <row r="15" ht="12.75" customHeight="1" s="6">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Wired Mouse</t>
@@ -510,7 +512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" ht="24" customHeight="1" s="6">
+    <row r="16" ht="12.75" customHeight="1" s="6">
       <c r="A16" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Wireless Headset Poly </t>
@@ -523,7 +525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" ht="24" customHeight="1" s="6">
+    <row r="17" ht="12.75" customHeight="1" s="6">
       <c r="A17" s="8" t="inlineStr">
         <is>
           <t>Wireless KB &amp; Mouse</t>
@@ -559,11 +561,11 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="18.29" customWidth="1" style="5" min="1" max="1"/>
     <col width="20.52" customWidth="1" style="5" min="2" max="2"/>
@@ -1120,7 +1122,7 @@
         </is>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="12.75" customHeight="1" s="6">
       <c r="A26" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 10:50:20</t>
@@ -1142,7 +1144,7 @@
         </is>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="12.75" customHeight="1" s="6">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 11:33:44</t>
@@ -1164,7 +1166,7 @@
         </is>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="12.75" customHeight="1" s="6">
       <c r="A28" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 12:35:48</t>
@@ -1186,7 +1188,7 @@
         </is>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="12.75" customHeight="1" s="6">
       <c r="A29" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 12:36:48</t>
@@ -1208,7 +1210,7 @@
         </is>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="12.75" customHeight="1" s="6">
       <c r="A30" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 12:41:56</t>
@@ -1230,7 +1232,7 @@
         </is>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="12.75" customHeight="1" s="6">
       <c r="A31" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 12:41:56</t>
@@ -1252,7 +1254,7 @@
         </is>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="12.75" customHeight="1" s="6">
       <c r="A32" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 12:41:57</t>
@@ -1274,29 +1276,29 @@
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="33" ht="12.75" customHeight="1" s="6">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 14:20:35</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
         <is>
           <t>subtract</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="5" t="inlineStr">
         <is>
           <t>SAN111111</t>
         </is>
       </c>
     </row>
-    <row r="1048576" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1321,10 +1323,10 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -1356,23 +1358,23 @@
         <v>19</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" ht="46.5" customHeight="1" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="6">
       <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="46.5" customHeight="1" s="6">
+    <row r="4" ht="12.75" customHeight="1" s="6">
       <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G2</t>
@@ -1385,7 +1387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" ht="35.25" customHeight="1" s="6">
+    <row r="5" ht="12.75" customHeight="1" s="6">
       <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G4</t>
@@ -1398,20 +1400,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="24" customHeight="1" s="6">
+    <row r="6" ht="12.75" customHeight="1" s="6">
       <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="B6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" ht="24" customHeight="1" s="6">
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="6">
       <c r="A7" s="8" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
@@ -1424,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" ht="24" customHeight="1" s="6">
+    <row r="8" ht="12.75" customHeight="1" s="6">
       <c r="A8" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Laptop Charger </t>
@@ -1437,7 +1439,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" ht="24" customHeight="1" s="6">
+    <row r="9" ht="12.75" customHeight="1" s="6">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
@@ -1456,10 +1458,14 @@
           <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
-      <c r="B10" s="7" t="n"/>
-      <c r="C10" s="7" t="n"/>
-    </row>
-    <row r="11" ht="24" customHeight="1" s="6">
+      <c r="B10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="6">
       <c r="A11" s="8" t="inlineStr">
         <is>
           <t>Monitor 34” Ultrawide</t>
@@ -1472,7 +1478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" ht="35.25" customHeight="1" s="6">
+    <row r="12" ht="12.75" customHeight="1" s="6">
       <c r="A12" s="8" t="inlineStr">
         <is>
           <t>USB DVD-RW Drive</t>
@@ -1485,7 +1491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" ht="35.25" customHeight="1" s="6">
+    <row r="13" ht="12.75" customHeight="1" s="6">
       <c r="A13" s="8" t="inlineStr">
         <is>
           <t>Wired Headset Poly</t>
@@ -1498,7 +1504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" ht="24" customHeight="1" s="6">
+    <row r="14" ht="12.75" customHeight="1" s="6">
       <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Wired Keyboard</t>
@@ -1511,7 +1517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" ht="24" customHeight="1" s="6">
+    <row r="15" ht="12.75" customHeight="1" s="6">
       <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Wired Mouse</t>
@@ -1524,7 +1530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" ht="35.25" customHeight="1" s="6">
+    <row r="16" ht="12.75" customHeight="1" s="6">
       <c r="A16" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">Wireless Headset Poly </t>
@@ -1563,13 +1569,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="18.56" customWidth="1" style="5" min="1" max="1"/>
     <col width="17.19" customWidth="1" style="5" min="2" max="2"/>
@@ -1952,6 +1958,50 @@
       <c r="D18" s="5" t="inlineStr">
         <is>
           <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="12.75" customHeight="1" s="6">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 14:28:23</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>SAN456123</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="12.75" customHeight="1" s="6">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 14:30:25</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
         </is>
       </c>
     </row>
@@ -1982,7 +2032,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -2220,15 +2270,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="25.36" customWidth="1" style="5" min="1" max="3"/>
+    <col width="25.36" customWidth="1" style="7" min="1" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="6">
@@ -2249,192 +2299,176 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="6">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>SAN456123</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:29:57</t>
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>SAN444555</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:30:30</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>SAN444555</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:30:30</t>
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>SAN456665</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:10</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="6">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Dock Thunderbolt G4</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>SAN456665</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:31:10</t>
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>SAN444444</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:19</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="6">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Wireless Headset Poly </t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>SAN444444</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:31:19</t>
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>SAN453212</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 10:31:27</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Laptop Charger </t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>SAN453212</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:31:27</t>
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>SAN122334</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:35:48</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="6">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>SAN343434</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 10:50:20</t>
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>SAN222211</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:36:48</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="6">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>SAN122334</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 12:35:48</t>
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>SAN456789</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
         </is>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="6">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>SAN222211</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 12:36:48</t>
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>SAN125689</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:56</t>
         </is>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="6">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>SAN456789</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 12:41:56</t>
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>SAN357895</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 12:41:57</t>
         </is>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="6">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>SAN125689</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 12:41:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1" s="6">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>SAN357895</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>2023-12-31 12:41:57</t>
-        </is>
-      </c>
-    </row>
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>SAN465768</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>2023-12-31 14:44:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="6"/>
     <row r="13" ht="12.75" customHeight="1" s="6"/>
     <row r="14" ht="12.75" customHeight="1" s="6"/>
     <row r="15" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Fixed logic of incorrect SAN alert not followed by the SAN Input box
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -307,7 +307,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -337,10 +337,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
@@ -559,13 +559,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="18.29" customWidth="1" style="5" min="1" max="1"/>
     <col width="20.52" customWidth="1" style="5" min="2" max="2"/>
@@ -1295,6 +1295,94 @@
       <c r="D33" s="5" t="inlineStr">
         <is>
           <t>SAN111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:04:39</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C34" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>SAN655443</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:05:19</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C35" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>SAN434343</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:08:18</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>SAN111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:08:38</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>SAN111444</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1414,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -1575,7 +1663,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="18.56" customWidth="1" style="5" min="1" max="1"/>
     <col width="17.19" customWidth="1" style="5" min="2" max="2"/>
@@ -2032,7 +2120,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="28" customWidth="1" style="5" min="1" max="1"/>
   </cols>
@@ -2270,13 +2358,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.36" customWidth="1" style="7" min="1" max="3"/>
   </cols>
@@ -2468,10 +2556,74 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="12.75" customHeight="1" s="6"/>
-    <row r="13" ht="12.75" customHeight="1" s="6"/>
-    <row r="14" ht="12.75" customHeight="1" s="6"/>
-    <row r="15" ht="12.75" customHeight="1" s="6"/>
+    <row r="12" ht="12.75" customHeight="1" s="6">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>SAN655443</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:04:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="6">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>SAN434343</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:05:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1" s="6">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SAN111111</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:08:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="12.75" customHeight="1" s="6">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SAN111444</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:08:38</t>
+        </is>
+      </c>
+    </row>
     <row r="16" ht="12.75" customHeight="1" s="6"/>
     <row r="17" ht="12.75" customHeight="1" s="6"/>
     <row r="18" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Ready for testing by others
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -337,10 +337,10 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
@@ -350,10 +350,10 @@
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="6">
@@ -363,10 +363,10 @@
         </is>
       </c>
       <c r="B4" s="7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="6">
@@ -376,10 +376,10 @@
         </is>
       </c>
       <c r="B5" s="7" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="6">
@@ -559,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
@@ -1343,48 +1343,146 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 16:08:18</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
+      <c r="B36" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
         <is>
           <t>SAN111111</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t>2023-12-31 16:08:38</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+      <c r="B37" s="5" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C37" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D37" s="5" t="inlineStr">
         <is>
           <t>SAN111444</t>
         </is>
       </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:15</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt Slim</t>
+        </is>
+      </c>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:24</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:39:27</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>SAN234567</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:39:30</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>SAN765432</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:39:41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="6"/>
   </sheetData>
@@ -1521,10 +1619,10 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="6">
@@ -1534,10 +1632,10 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="6">
@@ -1573,10 +1671,10 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="7" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="6">
@@ -1586,10 +1684,10 @@
         </is>
       </c>
       <c r="B13" s="7" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="6">
@@ -1599,10 +1697,10 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="6">
@@ -1612,10 +1710,10 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="6">
@@ -1657,7 +1755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -2090,6 +2188,100 @@
       <c r="D20" s="5" t="inlineStr">
         <is>
           <t>SAN343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:33</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>USB DVD-RW Drive</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:36</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:38</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:17:40</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Wired Mouse</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>2023-12-31 16:18:36</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>SAN434343,SAN655443</t>
         </is>
       </c>
     </row>
@@ -2564,12 +2756,12 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>SAN655443</t>
+          <t>SAN111111</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>2023-12-31 16:04:39</t>
+          <t>2023-12-31 16:08:18</t>
         </is>
       </c>
     </row>
@@ -2581,12 +2773,12 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>SAN434343</t>
+          <t>SAN111444</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>2023-12-31 16:05:19</t>
+          <t>2023-12-31 16:08:38</t>
         </is>
       </c>
     </row>
@@ -2598,12 +2790,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SAN111111</t>
+          <t>SAN234567</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-12-31 16:08:18</t>
+          <t>2023-12-31 16:39:27</t>
         </is>
       </c>
     </row>
@@ -2615,12 +2807,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SAN111444</t>
+          <t>SAN765432</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2023-12-31 16:08:38</t>
+          <t>2023-12-31 16:39:30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Comment out the "File" dropdown menu, and all submenu items. Bring the .XLSX button back to the main window.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Perth_Assets.xlsx
+++ b/Build Room/EUC_Perth_Assets.xlsx
@@ -328,7 +328,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="9" min="1" max="1"/>
   </cols>
@@ -579,13 +579,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="18.29" customWidth="1" style="9" min="1" max="1"/>
     <col width="20.52" customWidth="1" style="9" min="2" max="2"/>
@@ -2025,46 +2025,90 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="9" t="inlineStr">
         <is>
           <t>2024-01-03 21:44:59</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
+      <c r="B67" s="9" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C67" s="9" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D67" s="9" t="inlineStr">
         <is>
           <t>SAN147896</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="9" t="inlineStr">
         <is>
           <t>2024-01-03 21:45:07</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
+      <c r="B68" s="9" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C68" s="9" t="inlineStr">
         <is>
           <t>subtract</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D68" s="9" t="inlineStr">
         <is>
           <t>SAN147896</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="9" t="inlineStr">
+        <is>
+          <t>2024-01-10 19:22:14</t>
+        </is>
+      </c>
+      <c r="B69" s="9" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C69" s="9" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D69" s="9" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-01-11 20:15:00</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>SAN123432</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2140,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="9" min="1" max="1"/>
   </cols>
@@ -2345,7 +2389,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="18.56" customWidth="1" style="9" min="1" max="1"/>
     <col width="17.19" customWidth="1" style="9" min="2" max="2"/>
@@ -2927,7 +2971,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28" customWidth="1" style="9" min="1" max="1"/>
   </cols>
@@ -3165,13 +3209,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="25.36" customWidth="1" style="14" min="1" max="3"/>
   </cols>
@@ -3244,8 +3288,40 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1" s="12"/>
-    <row r="6" ht="12.75" customHeight="1" s="12"/>
+    <row r="5" ht="12.75" customHeight="1" s="12">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t>2024-01-10 19:22:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="12">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SAN123432</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-01-11 20:15:00</t>
+        </is>
+      </c>
+    </row>
     <row r="7" ht="12.75" customHeight="1" s="12"/>
     <row r="8" ht="12.75" customHeight="1" s="12"/>
     <row r="9" ht="12.75" customHeight="1" s="12"/>

</xml_diff>